<commit_message>
Path bug fixed on linux
</commit_message>
<xml_diff>
--- a/int4osemosys/data/OCGModel.xlsx
+++ b/int4osemosys/data/OCGModel.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20827"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CB1E215-58C3-48C6-B2D6-E13A1CA449AD}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2BDE873-C497-4363-92E3-07DA97DBA302}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1013" yWindow="0" windowWidth="7208" windowHeight="5430" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2033" yWindow="0" windowWidth="7208" windowHeight="5430" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Scenario Settings" sheetId="1" r:id="rId1"/>
@@ -2055,7 +2055,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
@@ -2650,8 +2650,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0E0EE79-6107-4FA4-A183-740D00DABDDE}">
   <dimension ref="A1:AE65"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="3" ySplit="3" topLeftCell="N57" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="3" ySplit="3" topLeftCell="N15" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
       <selection pane="bottomRight" activeCell="Q58" sqref="Q58"/>

</xml_diff>